<commit_message>
Fixed climate agg date sql
</commit_message>
<xml_diff>
--- a/ClimateAgreement_Data_RAW.xlsx
+++ b/ClimateAgreement_Data_RAW.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -488,8 +484,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>44502</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>to_date('2021-11-02 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -521,8 +519,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>44871</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-06 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -554,8 +554,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>44728</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>to_date('2022-06-16 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -587,8 +589,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>44498</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>to_date('2021-10-29 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -620,8 +624,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>44348</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>to_date('2021-06-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -655,7 +661,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>to_date('NULL', 'yyyy-mm-dd')</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,8 +694,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>45233</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>to_date('2023-11-03 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -723,7 +731,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>to_date('NULL', 'yyyy-mm-dd')</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -756,8 +764,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>44389</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>to_date('2021-07-12 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -791,7 +801,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>to_date('NULL', 'yyyy-mm-dd')</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -824,8 +834,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E12" s="2" t="n">
-        <v>43922</v>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>to_date('2020-04-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -857,8 +869,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>43922</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>to_date('2020-04-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -890,8 +904,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
-        <v>44497</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>to_date('2021-10-28 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -923,8 +939,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E15" s="2" t="n">
-        <v>44497</v>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>to_date('2021-10-28 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -956,8 +974,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>44195</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-30 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -989,8 +1009,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E17" s="2" t="n">
-        <v>44521</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>to_date('2021-11-21 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1022,8 +1044,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E18" s="2" t="n">
-        <v>44166</v>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1055,8 +1079,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E19" s="2" t="n">
-        <v>43800</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>to_date('2019-12-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1088,8 +1114,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E20" s="2" t="n">
-        <v>44400</v>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>to_date('2021-07-23 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1121,8 +1149,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
-        <v>44400</v>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>to_date('2021-07-23 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1154,8 +1184,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
-        <v>44426</v>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>to_date('2021-08-18 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1187,8 +1219,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>44426</v>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>to_date('2021-08-18 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1220,8 +1254,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E24" s="2" t="n">
-        <v>44799</v>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>to_date('2022-08-26 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1253,8 +1289,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E25" s="2" t="n">
-        <v>44799</v>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>to_date('2022-08-26 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1286,8 +1324,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n">
-        <v>44827</v>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>to_date('2022-09-23 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1319,8 +1359,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
-        <v>44827</v>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>to_date('2022-09-23 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1352,8 +1394,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E28" s="2" t="n">
-        <v>44369</v>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>to_date('2021-06-22 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1387,7 +1431,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>22/10/2021</t>
+          <t>to_date('22/10/2021', 'yyyy-mm-dd')</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1420,8 +1464,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E30" s="2" t="n">
-        <v>45104</v>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>to_date('2023-06-27 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1453,8 +1499,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>45104</v>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>to_date('2023-06-27 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1486,8 +1534,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E32" s="2" t="n">
-        <v>44193</v>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-28 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1519,8 +1569,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E33" s="2" t="n">
-        <v>44193</v>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-28 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1552,8 +1604,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E34" s="2" t="n">
-        <v>44882</v>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-17 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1585,8 +1639,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>44882</v>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-17 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1618,8 +1674,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>44369</v>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>to_date('2021-06-22 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1651,8 +1709,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E37" s="2" t="n">
-        <v>44369</v>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>to_date('2021-06-22 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1684,8 +1744,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>44166</v>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1717,8 +1779,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>44166</v>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1750,8 +1814,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>44407</v>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>to_date('2021-07-30 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1783,8 +1849,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>44407</v>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>to_date('2021-07-30 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1816,8 +1884,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
-        <v>44868</v>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-03 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1849,8 +1919,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E43" s="2" t="n">
-        <v>44160</v>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>to_date('2020-11-25 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1882,8 +1954,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E44" s="2" t="n">
-        <v>44183</v>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-18 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1915,8 +1989,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E45" s="2" t="n">
-        <v>44183</v>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>to_date('2020-12-18 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -1948,8 +2024,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E46" s="2" t="n">
-        <v>44301</v>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>to_date('2021-04-15 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1981,8 +2059,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E47" s="2" t="n">
-        <v>44301</v>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>to_date('2021-04-15 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2014,8 +2094,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E48" s="2" t="n">
-        <v>44869</v>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-04 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2047,8 +2129,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E49" s="2" t="n">
-        <v>44868</v>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-03 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2080,8 +2164,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E50" s="2" t="n">
-        <v>44547</v>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>to_date('2021-12-17 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2113,8 +2199,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E51" s="2" t="n">
-        <v>44224</v>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>to_date('2021-01-28 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2146,8 +2234,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E52" s="2" t="n">
-        <v>44867</v>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-02 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -2179,8 +2269,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E53" s="2" t="n">
-        <v>44867</v>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-02 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2212,8 +2304,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E54" s="2" t="n">
-        <v>45029</v>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>to_date('2023-04-13 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2245,8 +2339,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E55" s="2" t="n">
-        <v>44440</v>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>to_date('2021-09-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -2278,8 +2374,10 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E56" s="2" t="n">
-        <v>44572</v>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>to_date('2022-01-11 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2311,8 +2409,10 @@
           <t>Net Zero</t>
         </is>
       </c>
-      <c r="E57" s="2" t="n">
-        <v>44866</v>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>to_date('2022-11-01 ', 'yyyy-mm-dd')</t>
+        </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>

</xml_diff>